<commit_message>
se corrige error en el que se sumaba agrupación de dataframe en lugar de detectar el maximo
</commit_message>
<xml_diff>
--- a/downloads/Test.xlsx
+++ b/downloads/Test.xlsx
@@ -676,10 +676,10 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -690,10 +690,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -707,7 +707,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -758,10 +758,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -775,7 +775,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -789,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">

</xml_diff>